<commit_message>
Update of the spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes.xlsx
+++ b/spreadsheets/attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DD42810-E471-054E-B39F-9A34646F258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865E2E64-8EC8-444E-9D0B-E72A2EEAEEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="940" windowWidth="14900" windowHeight="16860" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>v 0.1</t>
   </si>
@@ -50,21 +50,12 @@
     <t>Date_of_measure</t>
   </si>
   <si>
-    <t>Exposure</t>
-  </si>
-  <si>
     <t>Dimensionnality_of_measure</t>
   </si>
   <si>
     <t>Sampling_Matrix_Size_(Nx,Ny,Nz)</t>
   </si>
   <si>
-    <t>Sampling_Step_Size_(dx,dy,dz)</t>
-  </si>
-  <si>
-    <t>Field_of_view_(X,Y,Z)</t>
-  </si>
-  <si>
     <t>SPECTROMETER</t>
   </si>
   <si>
@@ -77,9 +68,6 @@
     <t>Wavelength_nm</t>
   </si>
   <si>
-    <t>Confocal_Pinhole_Diameter</t>
-  </si>
-  <si>
     <t>Detection_Lens_NA</t>
   </si>
   <si>
@@ -95,54 +83,21 @@
     <t>Illumination_Lens_NA</t>
   </si>
   <si>
-    <t>Illumination_Power</t>
-  </si>
-  <si>
     <t>Illumination_Type</t>
   </si>
   <si>
     <t>Laser_Model</t>
   </si>
   <si>
-    <t>Laser_Drift</t>
-  </si>
-  <si>
     <t>Phonons_Measured</t>
   </si>
   <si>
     <t>Polarization_probed-analyzed</t>
   </si>
   <si>
-    <t>Scan_Amplitude</t>
-  </si>
-  <si>
     <t>Scanning_Strategy</t>
   </si>
   <si>
-    <t>Scattering_Angle</t>
-  </si>
-  <si>
-    <t>Spectral_Resolution</t>
-  </si>
-  <si>
-    <t>x-Mechanical_Resolution</t>
-  </si>
-  <si>
-    <t>x-Optical_Resolution</t>
-  </si>
-  <si>
-    <t>y-Mechanical_Resolution</t>
-  </si>
-  <si>
-    <t>y-Optical_Resolution</t>
-  </si>
-  <si>
-    <t>z-Mechanical_Resolution</t>
-  </si>
-  <si>
-    <t>z-Optical_Resolution</t>
-  </si>
-  <si>
     <t>FILEPROP</t>
   </si>
   <si>
@@ -281,9 +236,6 @@
     <t>Measured</t>
   </si>
   <si>
-    <t xml:space="preserve">Version of the spreadsheet </t>
-  </si>
-  <si>
     <t>Global name</t>
   </si>
   <si>
@@ -291,6 +243,57 @@
   </si>
   <si>
     <t>Water spectrum</t>
+  </si>
+  <si>
+    <t>Version of the spreadsheet - Don't change</t>
+  </si>
+  <si>
+    <t>v0.1</t>
+  </si>
+  <si>
+    <t>Exposure_s</t>
+  </si>
+  <si>
+    <t>Sampling_Step_Size_microm(dx,dy,dz)</t>
+  </si>
+  <si>
+    <t>Confocal_Pinhole_Diameter_AU</t>
+  </si>
+  <si>
+    <t>Field_Of_View_microm(X,Y,Z)</t>
+  </si>
+  <si>
+    <t>Illumination_Power_mW</t>
+  </si>
+  <si>
+    <t>Laser_Drift_MHz_per_h</t>
+  </si>
+  <si>
+    <t>Scan_Amplitude_GHz</t>
+  </si>
+  <si>
+    <t>Scattering_Angle_deg</t>
+  </si>
+  <si>
+    <t>Spectral_Resolution_MHz</t>
+  </si>
+  <si>
+    <t>x-Mechanical_Resolution_microm</t>
+  </si>
+  <si>
+    <t>x-Optical_Resolution_microm</t>
+  </si>
+  <si>
+    <t>y-Mechanical_Resolution_microm</t>
+  </si>
+  <si>
+    <t>y-Optical_Resolution_microm</t>
+  </si>
+  <si>
+    <t>z-Mechanical_Resolution_microm</t>
+  </si>
+  <si>
+    <t>z-Optical_Resolution_microm</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -713,10 +716,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -724,21 +727,21 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1">
         <v>0.1</v>
@@ -746,10 +749,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -757,73 +760,73 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
         <v>532</v>
@@ -831,10 +834,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -842,10 +845,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E17" s="1">
         <v>0.45</v>
@@ -853,63 +856,63 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1">
         <v>0.2</v>
@@ -917,13 +920,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E23" s="1">
         <v>15</v>
@@ -931,38 +934,38 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1">
         <v>700</v>
@@ -970,41 +973,41 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1">
         <v>20</v>
@@ -1012,24 +1015,24 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1">
         <v>180</v>
@@ -1037,13 +1040,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E32" s="1">
         <v>150</v>
@@ -1051,13 +1054,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E33" s="1">
         <v>0.5</v>
@@ -1065,13 +1068,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
@@ -1079,13 +1082,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E35" s="1">
         <v>0.5</v>
@@ -1093,13 +1096,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E36" s="1">
         <v>5</v>
@@ -1107,13 +1110,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E37" s="1">
         <v>0.5</v>
@@ -1121,13 +1124,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E38" s="1">
         <v>50</v>
@@ -1135,18 +1138,21 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E41" s="1">
         <v>0.1</v>
@@ -1154,27 +1160,27 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display of properties and export of Python code to access an element of the file
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes.xlsx
+++ b/spreadsheets/attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7116C8B8-37D3-994B-A6EC-B79F333B4292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB79DB7D-76EF-324F-B5A1-738F080E5EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes of a measure" sheetId="1" r:id="rId1"/>
@@ -210,9 +210,6 @@
     <t>MEASURE.Date_of_measure</t>
   </si>
   <si>
-    <t>MEASURE.Exposure_s</t>
-  </si>
-  <si>
     <t>MEASURE.Dimensionnality_of_measure</t>
   </si>
   <si>
@@ -222,24 +219,12 @@
     <t>MEASURE.Sampling_Matrix_Size_(Nx,Ny,Nz)</t>
   </si>
   <si>
-    <t>MEASURE.Sampling_Step_Size_microm(dx,dy,dz)</t>
-  </si>
-  <si>
-    <t>MEASURE.Field_Of_View_microm(X,Y,Z)</t>
-  </si>
-  <si>
     <t>SPECTROMETER.Type</t>
   </si>
   <si>
     <t>SPECTROMETER.Model</t>
   </si>
   <si>
-    <t>SPECTROMETER.Wavelength_nm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.Confocal_Pinhole_Diameter_AU</t>
-  </si>
-  <si>
     <t>SPECTROMETER.Detection_Lens_NA</t>
   </si>
   <si>
@@ -258,9 +243,6 @@
     <t>SPECTROMETER.Illumination_Lens_NA</t>
   </si>
   <si>
-    <t>SPECTROMETER.Illumination_Power_mW</t>
-  </si>
-  <si>
     <t>SPECTROMETER.Illumination_Type</t>
   </si>
   <si>
@@ -276,36 +258,9 @@
     <t>SPECTROMETER.Polarization_probed-analyzed</t>
   </si>
   <si>
-    <t>SPECTROMETER.Scan_Amplitude_GHz</t>
-  </si>
-  <si>
     <t>SPECTROMETER.Scanning_Strategy</t>
   </si>
   <si>
-    <t>SPECTROMETER.Scattering_Angle_deg</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.Spectral_Resolution_MHz</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.x-Mechanical_Resolution_microm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.x-Optical_Resolution_microm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.y-Mechanical_Resolution_microm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.y-Optical_Resolution_microm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.z-Mechanical_Resolution_microm</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.z-Optical_Resolution_microm</t>
-  </si>
-  <si>
     <t>FILEPROP.BLS_HDF5_Version</t>
   </si>
   <si>
@@ -313,6 +268,51 @@
   </si>
   <si>
     <t>FILEPROP.Name</t>
+  </si>
+  <si>
+    <t>MEASURE.Exposure_(s)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Wavelength_(nm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Confocal_Pinhole_Diameter_(AU)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Illumination_Power_(mW)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Scan_Amplitude_(GHz)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Scattering_Angle_(deg)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.Spectral_Resolution_(MHz)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.x-Mechanical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.x-Optical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.y-Mechanical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.y-Optical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.z-Mechanical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.z-Optical_Resolution_(microm)</t>
+  </si>
+  <si>
+    <t>MEASURE.Sampling_Step_Size_(dx,dy,dz)_(microm)</t>
+  </si>
+  <si>
+    <t>MEASURE.Field_Of_View_(X,Y,Z)_(microm)</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,7 +757,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
         <v>21</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Allows the drag and drop of CSV files to the attribute table view.
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes.xlsx
+++ b/spreadsheets/attributes.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB79DB7D-76EF-324F-B5A1-738F080E5EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114F407-2025-E042-A6DF-BE33D748803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes of a measure" sheetId="1" r:id="rId1"/>
-    <sheet name="Attributes of an element" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
   <si>
     <t>v 0.1</t>
   </si>
@@ -51,12 +50,6 @@
     <t>FILEPROP</t>
   </si>
   <si>
-    <t>Filepath</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -198,12 +191,6 @@
     <t>Global name of the h5 file</t>
   </si>
   <si>
-    <t>The global filepath to the original file</t>
-  </si>
-  <si>
-    <t>\Users\documents\spectra\raw_spectrum.dat</t>
-  </si>
-  <si>
     <t>MEASURE.Sample</t>
   </si>
   <si>
@@ -291,28 +278,28 @@
     <t>SPECTROMETER.Spectral_Resolution_(MHz)</t>
   </si>
   <si>
-    <t>SPECTROMETER.x-Mechanical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.x-Optical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.y-Mechanical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.y-Optical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.z-Mechanical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>SPECTROMETER.z-Optical_Resolution_(microm)</t>
-  </si>
-  <si>
-    <t>MEASURE.Sampling_Step_Size_(dx,dy,dz)_(microm)</t>
-  </si>
-  <si>
-    <t>MEASURE.Field_Of_View_(X,Y,Z)_(microm)</t>
+    <t>MEASURE.Sampling_Step_Size_(dx,dy,dz)_(µm)</t>
+  </si>
+  <si>
+    <t>MEASURE.Field_Of_View_(X,Y,Z)_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.x-Mechanical_Resolution_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.x-Optical_Resolution_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.y-Mechanical_Resolution_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.y-Optical_Resolution_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.z-Mechanical_Resolution_(µm)</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.z-Optical_Resolution_(µm)</t>
   </si>
 </sst>
 </file>
@@ -701,7 +688,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,13 +703,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -732,35 +719,35 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>0.1</v>
@@ -768,10 +755,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -779,46 +766,46 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -828,35 +815,35 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1">
         <v>532</v>
@@ -864,10 +851,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -875,10 +862,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18" s="1">
         <v>0.45</v>
@@ -886,63 +873,63 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
         <v>0.2</v>
@@ -950,13 +937,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1">
         <v>15</v>
@@ -964,38 +951,38 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1">
         <v>700</v>
@@ -1003,41 +990,41 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E30" s="1">
         <v>20</v>
@@ -1045,24 +1032,24 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E32" s="1">
         <v>180</v>
@@ -1070,13 +1057,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E33" s="1">
         <v>150</v>
@@ -1084,13 +1071,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E34" s="1">
         <v>0.5</v>
@@ -1098,13 +1085,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
@@ -1112,13 +1099,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E36" s="1">
         <v>0.5</v>
@@ -1126,13 +1113,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" s="1">
         <v>5</v>
@@ -1140,13 +1127,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1">
         <v>0.5</v>
@@ -1154,13 +1141,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E39" s="1">
         <v>50</v>
@@ -1173,16 +1160,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E42" s="1">
         <v>0.1</v>
@@ -1190,83 +1177,31 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10FF49C8-5C81-9E49-9207-DCFD249EB382}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>